<commit_message>
Added some html pages
Added join/create room(no functionality).
</commit_message>
<xml_diff>
--- a/excelTemplate.xlsx
+++ b/excelTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\website code\tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liann\Documents\LearnBlox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FD4CE39-A541-4AB2-A800-BF7779FA437A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0693EBAD-95B4-4378-BA44-4B42A2AF67FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1305" windowWidth="28800" windowHeight="14295" xr2:uid="{F0DD7BB8-89A6-4B49-8543-10F10976F8E7}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Option4</t>
   </si>
   <si>
-    <t>Correct Answer</t>
-  </si>
-  <si>
     <t>Who is the U.S. president?</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>Bush</t>
+  </si>
+  <si>
+    <t>Answer</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,29 +489,29 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -522,8 +522,8 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 F3:F1048576" xr:uid="{F8D7275A-2402-49BB-AB2B-2E6B579B219E}">
-      <formula1>B1:E1</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{F8D7275A-2402-49BB-AB2B-2E6B579B219E}">
+      <formula1>B3:E3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Error: Invalid Input. Use drop down menu to select answer." sqref="F2" xr:uid="{0C715988-3060-405B-960A-27B153F7360F}">
       <formula1>B2:E2</formula1>
@@ -534,15 +534,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100615E6551C83689459A2736858DC01C3E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ca5450f96ae9fe84e6d9e6754f6ec96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4cfe46ae-adc0-4018-8249-4f07f4fcacee" xmlns:ns4="9ac4e7e4-5b13-4b6f-8787-5134de57ec79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1b1a62964089ada276994219bb4e7ba" ns3:_="" ns4:_="">
     <xsd:import namespace="4cfe46ae-adc0-4018-8249-4f07f4fcacee"/>
@@ -765,6 +756,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -772,14 +772,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56B41337-5D2F-472D-8322-C0D33E489BF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBE39842-2E44-4884-BA11-DBEF90529C47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -798,6 +790,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56B41337-5D2F-472D-8322-C0D33E489BF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21760874-5791-4A88-8859-0E836678F682}">
   <ds:schemaRefs>

</xml_diff>